<commit_message>
EXERCICIO 4 - SE ENCADEADO
</commit_message>
<xml_diff>
--- a/[02]-exercicios-fatec/EXERCICIO 3 - EXCEL - CAIXA_01.xlsx
+++ b/[02]-exercicios-fatec/EXERCICIO 3 - EXCEL - CAIXA_01.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fatec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Programação em Microinformática\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7D3BEEC-6EC1-479C-97EA-B7F124BBFD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41463619-B2C9-48E4-8EA0-5658FD7037D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan1" sheetId="2" r:id="rId2"/>
     <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -390,11 +379,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="dd"/>
-    <numFmt numFmtId="167" formatCode="&quot;R$&quot;#,##0.00;[Red]&quot;R$&quot;\-#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd"/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;#,##0.00;[Red]&quot;R$&quot;\-#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -480,7 +469,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,6 +491,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -906,25 +907,25 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -933,14 +934,14 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -955,7 +956,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -968,8 +969,8 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -980,66 +981,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="7" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="7" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="7" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="7" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="7" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="8" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1057,6 +1048,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1341,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J306"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A40" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55:J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,17 +1357,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="A1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1442,7 +1440,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="76">
+      <c r="J4" s="66">
         <v>1259</v>
       </c>
     </row>
@@ -1479,7 +1477,7 @@
         <f>IF(C5=5,D5,0)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="77">
+      <c r="J5" s="67">
         <f>J4+E5-F5-G5-H5-I5</f>
         <v>1509</v>
       </c>
@@ -1517,7 +1515,7 @@
         <f t="shared" ref="I6:I48" si="4">IF(C6=5,D6,0)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="77">
+      <c r="J6" s="67">
         <f t="shared" ref="J6:J48" si="5">J5+E6-F6-G6-H6-I6</f>
         <v>1868</v>
       </c>
@@ -1555,7 +1553,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J7" s="77">
+      <c r="J7" s="67">
         <f t="shared" si="5"/>
         <v>2127</v>
       </c>
@@ -1593,7 +1591,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J8" s="77">
+      <c r="J8" s="67">
         <f t="shared" si="5"/>
         <v>2002</v>
       </c>
@@ -1631,7 +1629,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J9" s="77">
+      <c r="J9" s="67">
         <f t="shared" si="5"/>
         <v>1902</v>
       </c>
@@ -1669,7 +1667,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J10" s="77">
+      <c r="J10" s="67">
         <f t="shared" si="5"/>
         <v>2260</v>
       </c>
@@ -1707,7 +1705,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J11" s="77">
+      <c r="J11" s="67">
         <f t="shared" si="5"/>
         <v>2509</v>
       </c>
@@ -1745,7 +1743,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J12" s="77">
+      <c r="J12" s="67">
         <f t="shared" si="5"/>
         <v>2708</v>
       </c>
@@ -1783,7 +1781,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J13" s="77">
+      <c r="J13" s="67">
         <f t="shared" si="5"/>
         <v>1208</v>
       </c>
@@ -1821,7 +1819,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J14" s="77">
+      <c r="J14" s="67">
         <f t="shared" si="5"/>
         <v>858</v>
       </c>
@@ -1859,7 +1857,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J15" s="77">
+      <c r="J15" s="67">
         <f t="shared" si="5"/>
         <v>1077</v>
       </c>
@@ -1897,7 +1895,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J16" s="77">
+      <c r="J16" s="67">
         <f t="shared" si="5"/>
         <v>-1423</v>
       </c>
@@ -1935,7 +1933,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J17" s="77">
+      <c r="J17" s="67">
         <f t="shared" si="5"/>
         <v>-3273</v>
       </c>
@@ -1973,7 +1971,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J18" s="77">
+      <c r="J18" s="67">
         <f t="shared" si="5"/>
         <v>-4773</v>
       </c>
@@ -2011,7 +2009,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J19" s="77">
+      <c r="J19" s="67">
         <f t="shared" si="5"/>
         <v>-6273</v>
       </c>
@@ -2049,7 +2047,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J20" s="77">
+      <c r="J20" s="67">
         <f t="shared" si="5"/>
         <v>-6423</v>
       </c>
@@ -2087,7 +2085,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J21" s="77">
+      <c r="J21" s="67">
         <f t="shared" si="5"/>
         <v>-6490.8</v>
       </c>
@@ -2125,7 +2123,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J22" s="77">
+      <c r="J22" s="67">
         <f t="shared" si="5"/>
         <v>-8990.7999999999993</v>
       </c>
@@ -2163,7 +2161,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J23" s="77">
+      <c r="J23" s="67">
         <f t="shared" si="5"/>
         <v>-9090.6999999999989</v>
       </c>
@@ -2201,7 +2199,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J24" s="77">
+      <c r="J24" s="67">
         <f t="shared" si="5"/>
         <v>-9209.6999999999989</v>
       </c>
@@ -2239,7 +2237,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J25" s="77">
+      <c r="J25" s="67">
         <f t="shared" si="5"/>
         <v>-9648.6999999999989</v>
       </c>
@@ -2277,7 +2275,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J26" s="77">
+      <c r="J26" s="67">
         <f t="shared" si="5"/>
         <v>-9808.6999999999989</v>
       </c>
@@ -2315,7 +2313,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J27" s="77">
+      <c r="J27" s="67">
         <f t="shared" si="5"/>
         <v>-9549.6999999999989</v>
       </c>
@@ -2353,7 +2351,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J28" s="77">
+      <c r="J28" s="67">
         <f t="shared" si="5"/>
         <v>-9200.6999999999989</v>
       </c>
@@ -2391,7 +2389,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J29" s="77">
+      <c r="J29" s="67">
         <f t="shared" si="5"/>
         <v>-8981.6999999999989</v>
       </c>
@@ -2429,7 +2427,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J30" s="77">
+      <c r="J30" s="67">
         <f t="shared" si="5"/>
         <v>-9060.6999999999989</v>
       </c>
@@ -2467,7 +2465,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J31" s="77">
+      <c r="J31" s="67">
         <f t="shared" si="5"/>
         <v>-9120.619999999999</v>
       </c>
@@ -2505,8 +2503,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J32" s="77">
-        <f t="shared" si="5"/>
+      <c r="J32" s="67">
+        <f>J31+E32-F32-G32-H32-I32</f>
         <v>-9144.619999999999</v>
       </c>
     </row>
@@ -2543,7 +2541,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J33" s="77">
+      <c r="J33" s="67">
         <f t="shared" si="5"/>
         <v>-9524.619999999999</v>
       </c>
@@ -2581,7 +2579,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J34" s="77">
+      <c r="J34" s="67">
         <f t="shared" si="5"/>
         <v>-9305.619999999999</v>
       </c>
@@ -2619,7 +2617,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J35" s="77">
+      <c r="J35" s="67">
         <f t="shared" si="5"/>
         <v>-9355.619999999999</v>
       </c>
@@ -2657,7 +2655,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J36" s="77">
+      <c r="J36" s="67">
         <f t="shared" si="5"/>
         <v>-9036.619999999999</v>
       </c>
@@ -2695,7 +2693,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J37" s="77">
+      <c r="J37" s="67">
         <f t="shared" si="5"/>
         <v>-9586.619999999999</v>
       </c>
@@ -2733,7 +2731,7 @@
         <f t="shared" si="4"/>
         <v>1500</v>
       </c>
-      <c r="J38" s="77">
+      <c r="J38" s="67">
         <f t="shared" si="5"/>
         <v>-11086.619999999999</v>
       </c>
@@ -2771,7 +2769,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J39" s="77">
+      <c r="J39" s="67">
         <f t="shared" si="5"/>
         <v>-11206.619999999999</v>
       </c>
@@ -2809,7 +2807,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J40" s="77">
+      <c r="J40" s="67">
         <f t="shared" si="5"/>
         <v>-11261.619999999999</v>
       </c>
@@ -2847,7 +2845,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J41" s="77">
+      <c r="J41" s="67">
         <f t="shared" si="5"/>
         <v>-7761.619999999999</v>
       </c>
@@ -2885,7 +2883,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J42" s="77">
+      <c r="J42" s="67">
         <f t="shared" si="5"/>
         <v>-7786.619999999999</v>
       </c>
@@ -2923,7 +2921,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J43" s="77">
+      <c r="J43" s="67">
         <f t="shared" si="5"/>
         <v>-7885.619999999999</v>
       </c>
@@ -2961,7 +2959,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J44" s="77">
+      <c r="J44" s="67">
         <f t="shared" si="5"/>
         <v>-7985.619999999999</v>
       </c>
@@ -2999,7 +2997,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J45" s="77">
+      <c r="J45" s="67">
         <f t="shared" si="5"/>
         <v>-8105.619999999999</v>
       </c>
@@ -3037,7 +3035,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J46" s="77">
+      <c r="J46" s="67">
         <f t="shared" si="5"/>
         <v>-8355.619999999999</v>
       </c>
@@ -3075,7 +3073,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J47" s="77">
+      <c r="J47" s="67">
         <f t="shared" si="5"/>
         <v>-8424.619999999999</v>
       </c>
@@ -3113,7 +3111,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J48" s="77">
+      <c r="J48" s="67">
         <f t="shared" si="5"/>
         <v>-8574.619999999999</v>
       </c>
@@ -3123,11 +3121,11 @@
       <c r="B49" s="15"/>
       <c r="C49" s="22"/>
       <c r="D49" s="41"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="60"/>
-      <c r="H49" s="60"/>
-      <c r="I49" s="61"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="60"/>
       <c r="J49" s="49"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3136,27 +3134,27 @@
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="42"/>
-      <c r="E50" s="71">
-        <f t="shared" ref="D50:I50" si="6">SUM(E5:E48)</f>
+      <c r="E50" s="82">
+        <f t="shared" ref="E50:I50" si="6">SUM(E5:E48)</f>
         <v>6758</v>
       </c>
-      <c r="F50" s="68">
+      <c r="F50" s="77">
         <f t="shared" si="6"/>
         <v>8850</v>
       </c>
-      <c r="G50" s="66">
+      <c r="G50" s="78">
         <f t="shared" si="6"/>
         <v>4384.82</v>
       </c>
-      <c r="H50" s="63">
+      <c r="H50" s="79">
         <f t="shared" si="6"/>
         <v>1856.8</v>
       </c>
-      <c r="I50" s="73">
+      <c r="I50" s="80">
         <f t="shared" si="6"/>
         <v>1500</v>
       </c>
-      <c r="J50" s="74"/>
+      <c r="J50" s="65"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="17" t="s">
@@ -3164,35 +3162,35 @@
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="42"/>
-      <c r="E51" s="72">
-        <f>E50/D54</f>
-        <v>0.28942655169548798</v>
-      </c>
-      <c r="F51" s="70">
-        <f>F50/D54</f>
-        <v>0.37902115751776688</v>
-      </c>
-      <c r="G51" s="67">
-        <f>G50/D54</f>
-        <v>0.18778977987650333</v>
+      <c r="E51" s="64">
+        <f>E50/D53</f>
+        <v>1</v>
+      </c>
+      <c r="F51" s="64">
+        <f t="shared" ref="F51:I51" si="7">F50/$D$54</f>
+        <v>0.53340180163239037</v>
+      </c>
+      <c r="G51" s="64">
+        <f t="shared" si="7"/>
+        <v>0.2642791963653941</v>
       </c>
       <c r="H51" s="64">
-        <f>H50/D54</f>
-        <v>7.9521636754688083E-2</v>
-      </c>
-      <c r="I51" s="75">
-        <f>I50/D54</f>
-        <v>6.4240874155553712E-2</v>
-      </c>
-      <c r="J51" s="74"/>
+        <f t="shared" si="7"/>
+        <v>0.11191191697977654</v>
+      </c>
+      <c r="I51" s="64">
+        <f t="shared" si="7"/>
+        <v>9.0407085022439049E-2</v>
+      </c>
+      <c r="J51" s="65"/>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="51"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="69"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="65"/>
-      <c r="I52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="63"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="61"/>
       <c r="J52" s="50"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3200,7 +3198,7 @@
         <v>61</v>
       </c>
       <c r="C53" s="53"/>
-      <c r="D53" s="54">
+      <c r="D53" s="83">
         <f>E50</f>
         <v>6758</v>
       </c>
@@ -3216,9 +3214,9 @@
         <v>62</v>
       </c>
       <c r="C54" s="53"/>
-      <c r="D54" s="54">
-        <f>SUM(E50:I50)</f>
-        <v>23349.62</v>
+      <c r="D54" s="81">
+        <f>SUM(F50:I50)</f>
+        <v>16591.62</v>
       </c>
       <c r="E54" s="52"/>
       <c r="F54" s="45"/>
@@ -3231,23 +3229,23 @@
       <c r="B55" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="55"/>
-      <c r="D55" s="56">
-        <f>J48</f>
+      <c r="C55" s="54"/>
+      <c r="D55" s="55">
+        <f>D53+J4-D54</f>
         <v>-8574.619999999999</v>
       </c>
       <c r="E55" s="52"/>
       <c r="F55" s="45"/>
-      <c r="G55" s="80"/>
-      <c r="H55" s="80"/>
-      <c r="I55" s="80"/>
-      <c r="J55" s="81"/>
+      <c r="G55" s="70"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
+      <c r="J55" s="71"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
-      <c r="D56" s="57"/>
+      <c r="D56" s="56"/>
       <c r="E56" s="28"/>
       <c r="F56" s="28"/>
       <c r="G56" s="28"/>
@@ -3599,6 +3597,7 @@
     <mergeCell ref="G55:J55"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -3607,7 +3606,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3615,7 +3614,7 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
@@ -3639,11 +3638,11 @@
       <c r="E1" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="84"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -3843,11 +3842,11 @@
       <c r="E1" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -3864,9 +3863,9 @@
         <v>0.5</v>
       </c>
       <c r="E2" s="24"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
@@ -3883,9 +3882,9 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="E3" s="24"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
@@ -3902,9 +3901,9 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="E4" s="24"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
@@ -3921,9 +3920,9 @@
         <v>0.05</v>
       </c>
       <c r="E5" s="24"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
@@ -3940,9 +3939,9 @@
         <v>0.06</v>
       </c>
       <c r="E6" s="24"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
@@ -3959,9 +3958,9 @@
         <v>0.05</v>
       </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
@@ -3978,9 +3977,9 @@
         <v>1.4285714285714285E-2</v>
       </c>
       <c r="E8" s="24"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
@@ -3997,23 +3996,23 @@
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E9" s="24"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="86" t="s">
+      <c r="A11" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="86"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
+      <c r="B11" s="76"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
@@ -4022,9 +4021,9 @@
       <c r="B12" s="24">
         <v>10</v>
       </c>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
@@ -4033,9 +4032,9 @@
       <c r="B13" s="24">
         <v>20</v>
       </c>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">

</xml_diff>